<commit_message>
1. Added Link Column with complete functionality 2. Added Search functionality
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>dhiraj</t>
+  </si>
+  <si>
+    <t>suvarna</t>
   </si>
 </sst>
 </file>
@@ -357,7 +360,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>